<commit_message>
Early GPU rendering, colour modification and upscaling.
</commit_message>
<xml_diff>
--- a/Documentation/GraphicsModes.xlsx
+++ b/Documentation/GraphicsModes.xlsx
@@ -163,7 +163,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -202,16 +202,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -547,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2332A2-3074-4648-AFA2-D28A6BF7FB4B}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +616,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>80</v>
@@ -638,7 +628,7 @@
         <v>8</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6" si="0">(C6*D6*E6*$C$4)/8</f>
+        <f>(C6*D6*E6*$C$4)/8</f>
         <v>4000</v>
       </c>
       <c r="G6" s="4">
@@ -662,7 +652,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>80</v>
@@ -674,19 +664,19 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F34" si="1">(C7*D7*E7*$C$4)/8</f>
+        <f t="shared" ref="F7:F34" si="0">(C7*D7*E7*$C$4)/8</f>
         <v>2000</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" ref="G7:G34" si="2">$B$1/C7</f>
+        <f t="shared" ref="G7:G34" si="1">$B$1/C7</f>
         <v>8</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" ref="H7:H34" si="3">$C$1/D7</f>
+        <f t="shared" ref="H7:H34" si="2">$C$1/D7</f>
         <v>8</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I34" si="4">$B$2-F7</f>
+        <f t="shared" ref="I7:I34" si="3">$B$2-F7</f>
         <v>63536</v>
       </c>
       <c r="J7">
@@ -698,7 +688,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>80</v>
@@ -710,19 +700,19 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="I8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>64536</v>
       </c>
       <c r="J8">
@@ -733,8 +723,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
-        <v>13</v>
+      <c r="B9">
+        <v>8</v>
       </c>
       <c r="C9" s="5">
         <v>80</v>
@@ -746,19 +736,19 @@
         <v>1</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="H9" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="I9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>65036</v>
       </c>
       <c r="J9">
@@ -770,7 +760,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>128</v>
@@ -782,25 +772,25 @@
         <v>8</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10240</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>55296</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>128</v>
@@ -812,25 +802,25 @@
         <v>4</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5120</v>
       </c>
       <c r="G11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>60416</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>128</v>
@@ -842,25 +832,25 @@
         <v>2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2560</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>62976</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="5">
-        <v>17</v>
+      <c r="B13">
+        <v>12</v>
       </c>
       <c r="C13" s="5">
         <v>128</v>
@@ -872,25 +862,25 @@
         <v>1</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1280</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>64256</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>160</v>
@@ -902,25 +892,25 @@
         <v>8</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12800</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>52736</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>160</v>
@@ -932,25 +922,25 @@
         <v>4</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6400</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>59136</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>160</v>
@@ -962,25 +952,25 @@
         <v>2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3200</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>62336</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="5">
-        <v>21</v>
+      <c r="B17">
+        <v>16</v>
       </c>
       <c r="C17" s="5">
         <v>160</v>
@@ -992,25 +982,25 @@
         <v>1</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>63936</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>160</v>
@@ -1022,25 +1012,25 @@
         <v>8</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16000</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>49536</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>160</v>
@@ -1052,25 +1042,25 @@
         <v>4</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8000</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>57536</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>160</v>
@@ -1082,25 +1072,25 @@
         <v>2</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4000</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>61536</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="5">
-        <v>25</v>
+      <c r="B21">
+        <v>20</v>
       </c>
       <c r="C21" s="5">
         <v>160</v>
@@ -1112,25 +1102,25 @@
         <v>1</v>
       </c>
       <c r="F21" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="G21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>63536</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>320</v>
@@ -1142,25 +1132,25 @@
         <v>8</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32000</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33536</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>320</v>
@@ -1172,25 +1162,25 @@
         <v>4</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16000</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>49536</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>320</v>
@@ -1202,25 +1192,25 @@
         <v>2</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8000</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>57536</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="5">
-        <v>29</v>
+      <c r="B25">
+        <v>24</v>
       </c>
       <c r="C25" s="5">
         <v>320</v>
@@ -1232,25 +1222,25 @@
         <v>1</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4000</v>
       </c>
       <c r="G25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>61536</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C26">
         <v>320</v>
@@ -1262,25 +1252,25 @@
         <v>8</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>64000</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1536</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>320</v>
@@ -1292,25 +1282,25 @@
         <v>4</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32000</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33536</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>320</v>
@@ -1322,25 +1312,25 @@
         <v>2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16000</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>49536</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="5">
-        <v>33</v>
+      <c r="B29">
+        <v>28</v>
       </c>
       <c r="C29" s="5">
         <v>320</v>
@@ -1352,25 +1342,25 @@
         <v>1</v>
       </c>
       <c r="F29" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8000</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H29" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>57536</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>640</v>
@@ -1382,25 +1372,25 @@
         <v>4</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>64000</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1536</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>640</v>
@@ -1412,25 +1402,25 @@
         <v>2</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32000</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33536</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="5">
-        <v>36</v>
+      <c r="B32">
+        <v>31</v>
       </c>
       <c r="C32" s="5">
         <v>640</v>
@@ -1442,25 +1432,25 @@
         <v>1</v>
       </c>
       <c r="F32" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16000</v>
       </c>
       <c r="G32" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H32" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>49536</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>640</v>
@@ -1472,25 +1462,25 @@
         <v>2</v>
       </c>
       <c r="F33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>64000</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1536</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>640</v>
@@ -1502,19 +1492,19 @@
         <v>1</v>
       </c>
       <c r="F34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32000</v>
       </c>
       <c r="G34" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H34" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33536</v>
       </c>
     </row>
@@ -1619,11 +1609,11 @@
         <v>4000</v>
       </c>
       <c r="G40">
-        <f t="shared" ref="G40:G43" si="5">C40*$G$37</f>
+        <f t="shared" ref="G40:G43" si="4">C40*$G$37</f>
         <v>320</v>
       </c>
       <c r="H40">
-        <f t="shared" ref="H40:H43" si="6">D40*$G$37</f>
+        <f t="shared" ref="H40:H43" si="5">D40*$G$37</f>
         <v>200</v>
       </c>
       <c r="I40">
@@ -1635,7 +1625,7 @@
         <v>2</v>
       </c>
       <c r="K40">
-        <f t="shared" ref="K40:K43" si="7">$B$2-F40</f>
+        <f t="shared" ref="K40:K43" si="6">$B$2-F40</f>
         <v>61536</v>
       </c>
     </row>
@@ -1657,11 +1647,11 @@
         <v>4000</v>
       </c>
       <c r="G41">
+        <f t="shared" si="4"/>
+        <v>640</v>
+      </c>
+      <c r="H41">
         <f t="shared" si="5"/>
-        <v>640</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="I41">
@@ -1673,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="K41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>61536</v>
       </c>
     </row>
@@ -1695,11 +1685,11 @@
         <v>8000</v>
       </c>
       <c r="G42">
+        <f t="shared" si="4"/>
+        <v>640</v>
+      </c>
+      <c r="H42">
         <f t="shared" si="5"/>
-        <v>640</v>
-      </c>
-      <c r="H42">
-        <f t="shared" si="6"/>
         <v>400</v>
       </c>
       <c r="I42">
@@ -1711,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="K42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>57536</v>
       </c>
     </row>
@@ -1733,11 +1723,11 @@
         <v>4000</v>
       </c>
       <c r="G43">
+        <f t="shared" si="4"/>
+        <v>640</v>
+      </c>
+      <c r="H43">
         <f t="shared" si="5"/>
-        <v>640</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="6"/>
         <v>400</v>
       </c>
       <c r="I43">
@@ -1749,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="K43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>61536</v>
       </c>
     </row>
@@ -1760,7 +1750,7 @@
     <mergeCell ref="G38:H38"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:F34">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
       <formula>$B$2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Gpu Layer drawing, bitmap drawing, and scanline colour registers
</commit_message>
<xml_diff>
--- a/Documentation/GraphicsModes.xlsx
+++ b/Documentation/GraphicsModes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -535,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2332A2-3074-4648-AFA2-D28A6BF7FB4B}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,19 +664,19 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F34" si="0">(C7*D7*E7*$C$4)/8</f>
+        <f t="shared" ref="F7:F29" si="0">(C7*D7*E7*$C$4)/8</f>
         <v>2000</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" ref="G7:G34" si="1">$B$1/C7</f>
+        <f t="shared" ref="G7:G29" si="1">$B$1/C7</f>
         <v>8</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" ref="H7:H34" si="2">$C$1/D7</f>
+        <f t="shared" ref="H7:H29" si="2">$C$1/D7</f>
         <v>8</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I34" si="3">$B$2-F7</f>
+        <f t="shared" ref="I7:I29" si="3">$B$2-F7</f>
         <v>63536</v>
       </c>
       <c r="J7">
@@ -769,11 +769,11 @@
         <v>80</v>
       </c>
       <c r="E10">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>10240</v>
+        <v>5120</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="1"/>
@@ -785,7 +785,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>55296</v>
+        <v>60416</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -799,11 +799,11 @@
         <v>80</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>5120</v>
+        <v>2560</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="1"/>
@@ -815,67 +815,67 @@
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>60416</v>
+        <v>62976</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>128</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>80</v>
       </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>2560</v>
-      </c>
-      <c r="G12" s="4">
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>1280</v>
+      </c>
+      <c r="G12" s="6">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="6">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>62976</v>
+        <v>64256</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="5">
-        <v>128</v>
-      </c>
-      <c r="D13" s="5">
+      <c r="C13">
+        <v>160</v>
+      </c>
+      <c r="D13">
         <v>80</v>
       </c>
-      <c r="E13" s="5">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5">
-        <f t="shared" si="0"/>
-        <v>1280</v>
-      </c>
-      <c r="G13" s="6">
-        <f t="shared" si="1"/>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>6400</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H13" s="6">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>64256</v>
+        <v>59136</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -889,11 +889,11 @@
         <v>80</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>12800</v>
+        <v>3200</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="1"/>
@@ -905,37 +905,37 @@
       </c>
       <c r="I14">
         <f t="shared" si="3"/>
-        <v>52736</v>
+        <v>62336</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>160</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <v>80</v>
       </c>
-      <c r="E15">
-        <v>4</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>6400</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H15" s="4">
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H15" s="6">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I15">
         <f t="shared" si="3"/>
-        <v>59136</v>
+        <v>63936</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -946,14 +946,14 @@
         <v>160</v>
       </c>
       <c r="D16">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>3200</v>
+        <v>8000</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" si="1"/>
@@ -961,79 +961,79 @@
       </c>
       <c r="H16" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I16">
         <f t="shared" si="3"/>
-        <v>62336</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+        <v>57536</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17">
         <v>160</v>
       </c>
-      <c r="D17" s="5">
-        <v>80</v>
-      </c>
-      <c r="E17" s="5">
-        <v>1</v>
-      </c>
-      <c r="F17" s="5">
-        <f t="shared" si="0"/>
-        <v>1600</v>
-      </c>
-      <c r="G17" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H17" s="6">
-        <f t="shared" si="2"/>
-        <v>5</v>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
-        <v>63936</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+        <v>61536</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="5">
         <v>160</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="5">
         <v>100</v>
       </c>
-      <c r="E18">
-        <v>8</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>16000</v>
-      </c>
-      <c r="G18" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H18" s="4">
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H18" s="6">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
-        <v>49536</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+        <v>63536</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D19">
         <v>100</v>
@@ -1043,11 +1043,11 @@
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>16000</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19" s="4">
         <f t="shared" si="2"/>
@@ -1055,15 +1055,15 @@
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>57536</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+        <v>49536</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D20">
         <v>100</v>
@@ -1073,11 +1073,11 @@
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H20" s="4">
         <f t="shared" si="2"/>
@@ -1085,15 +1085,15 @@
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
-        <v>61536</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+        <v>57536</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" s="5">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D21" s="5">
         <v>100</v>
@@ -1103,11 +1103,11 @@
       </c>
       <c r="F21" s="5">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="G21" s="6">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H21" s="6">
         <f t="shared" si="2"/>
@@ -1115,10 +1115,10 @@
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>63536</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+        <v>61536</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>21</v>
       </c>
@@ -1126,10 +1126,10 @@
         <v>320</v>
       </c>
       <c r="D22">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
@@ -1141,14 +1141,14 @@
       </c>
       <c r="H22" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
         <v>33536</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>22</v>
       </c>
@@ -1156,10 +1156,10 @@
         <v>320</v>
       </c>
       <c r="D23">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
@@ -1171,93 +1171,93 @@
       </c>
       <c r="H23" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I23">
         <f t="shared" si="3"/>
         <v>49536</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>23</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="5">
         <v>320</v>
       </c>
-      <c r="D24">
-        <v>100</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-      <c r="F24">
+      <c r="D24" s="5">
+        <v>200</v>
+      </c>
+      <c r="E24" s="5">
+        <v>1</v>
+      </c>
+      <c r="F24" s="5">
         <f t="shared" si="0"/>
         <v>8000</v>
       </c>
-      <c r="G24" s="4">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H24" s="4">
-        <f t="shared" si="2"/>
-        <v>4</v>
+      <c r="G24" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H24" s="6">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="I24">
         <f t="shared" si="3"/>
         <v>57536</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>24</v>
       </c>
-      <c r="C25" s="5">
-        <v>320</v>
-      </c>
-      <c r="D25" s="5">
-        <v>100</v>
-      </c>
-      <c r="E25" s="5">
-        <v>1</v>
-      </c>
-      <c r="F25" s="5">
-        <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="G25" s="6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H25" s="6">
-        <f t="shared" si="2"/>
-        <v>4</v>
+      <c r="C25">
+        <v>640</v>
+      </c>
+      <c r="D25">
+        <v>200</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>64000</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="I25">
         <f t="shared" si="3"/>
-        <v>61536</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26">
-        <v>320</v>
+        <v>640</v>
       </c>
       <c r="D26">
         <v>200</v>
       </c>
       <c r="E26">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>64000</v>
+        <v>32000</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" s="4">
         <f t="shared" si="2"/>
@@ -1265,480 +1265,330 @@
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+        <v>33536</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>26</v>
       </c>
-      <c r="C27">
-        <v>320</v>
-      </c>
-      <c r="D27">
+      <c r="C27" s="5">
+        <v>640</v>
+      </c>
+      <c r="D27" s="5">
         <v>200</v>
       </c>
-      <c r="E27">
-        <v>4</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="0"/>
-        <v>32000</v>
-      </c>
-      <c r="G27" s="4">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H27" s="4">
+      <c r="E27" s="5">
+        <v>1</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="0"/>
+        <v>16000</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H27" s="6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I27">
         <f t="shared" si="3"/>
-        <v>33536</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+        <v>49536</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>27</v>
       </c>
       <c r="C28">
-        <v>320</v>
+        <v>640</v>
       </c>
       <c r="D28">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>16000</v>
+        <v>64000</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H28" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28">
         <f t="shared" si="3"/>
-        <v>49536</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>28</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29">
+        <v>640</v>
+      </c>
+      <c r="D29">
+        <v>400</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>32000</v>
+      </c>
+      <c r="G29" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="3"/>
+        <v>33536</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1">
+        <v>8</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="1">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="7"/>
+      <c r="K33" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>20</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+      <c r="F34">
+        <f>(C34*D34*E34*$C$32)/8</f>
+        <v>800</v>
+      </c>
+      <c r="G34">
+        <f>C34*$G$32</f>
+        <v>160</v>
+      </c>
+      <c r="H34">
+        <f>D34*$G$32</f>
+        <v>80</v>
+      </c>
+      <c r="I34">
+        <f>$B$1/G34</f>
+        <v>4</v>
+      </c>
+      <c r="J34">
+        <f>$C$1/H34</f>
+        <v>5</v>
+      </c>
+      <c r="K34">
+        <f>$B$2-F34</f>
+        <v>64736</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>40</v>
+      </c>
+      <c r="D35">
+        <v>25</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <f>(C35*D35*E35*$C$32)/8</f>
+        <v>4000</v>
+      </c>
+      <c r="G35">
+        <f t="shared" ref="G35:G38" si="4">C35*$G$32</f>
         <v>320</v>
       </c>
-      <c r="D29" s="5">
+      <c r="H35">
+        <f t="shared" ref="H35:H38" si="5">D35*$G$32</f>
         <v>200</v>
       </c>
-      <c r="E29" s="5">
-        <v>1</v>
-      </c>
-      <c r="F29" s="5">
-        <f t="shared" si="0"/>
-        <v>8000</v>
-      </c>
-      <c r="G29" s="6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H29" s="6">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="3"/>
-        <v>57536</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>29</v>
-      </c>
-      <c r="C30">
-        <v>640</v>
-      </c>
-      <c r="D30">
-        <v>200</v>
-      </c>
-      <c r="E30">
-        <v>4</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="0"/>
-        <v>64000</v>
-      </c>
-      <c r="G30" s="4">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H30" s="4">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="3"/>
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>30</v>
-      </c>
-      <c r="C31">
-        <v>640</v>
-      </c>
-      <c r="D31">
-        <v>200</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="0"/>
-        <v>32000</v>
-      </c>
-      <c r="G31" s="4">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H31" s="4">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="3"/>
-        <v>33536</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>31</v>
-      </c>
-      <c r="C32" s="5">
-        <v>640</v>
-      </c>
-      <c r="D32" s="5">
-        <v>200</v>
-      </c>
-      <c r="E32" s="5">
-        <v>1</v>
-      </c>
-      <c r="F32" s="5">
-        <f t="shared" si="0"/>
-        <v>16000</v>
-      </c>
-      <c r="G32" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H32" s="6">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="3"/>
-        <v>49536</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>32</v>
-      </c>
-      <c r="C33">
-        <v>640</v>
-      </c>
-      <c r="D33">
-        <v>400</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="0"/>
-        <v>64000</v>
-      </c>
-      <c r="G33" s="4">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H33" s="4">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="3"/>
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>33</v>
-      </c>
-      <c r="C34">
-        <v>640</v>
-      </c>
-      <c r="D34">
-        <v>400</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="0"/>
-        <v>32000</v>
-      </c>
-      <c r="G34" s="4">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H34" s="4">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="3"/>
-        <v>33536</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="1">
-        <v>8</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="1">
-        <v>8</v>
-      </c>
-      <c r="H37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J38" s="7"/>
-      <c r="K38" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>20</v>
-      </c>
-      <c r="D39">
-        <v>10</v>
-      </c>
-      <c r="E39">
-        <v>4</v>
-      </c>
-      <c r="F39">
-        <f>(C39*D39*E39*$C$37)/8</f>
-        <v>800</v>
-      </c>
-      <c r="G39">
-        <f>C39*$G$37</f>
-        <v>160</v>
-      </c>
-      <c r="H39">
-        <f>D39*$G$37</f>
+      <c r="I35">
+        <f>$B$1/G35</f>
+        <v>2</v>
+      </c>
+      <c r="J35">
+        <f>$C$1/H35</f>
+        <v>2</v>
+      </c>
+      <c r="K35">
+        <f t="shared" ref="K35:K38" si="6">$B$2-F35</f>
+        <v>61536</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
         <v>80</v>
       </c>
-      <c r="I39">
-        <f>$B$1/G39</f>
-        <v>4</v>
-      </c>
-      <c r="J39">
-        <f>$C$1/H39</f>
-        <v>5</v>
-      </c>
-      <c r="K39">
-        <f>$B$2-F39</f>
-        <v>64736</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>40</v>
-      </c>
-      <c r="D40">
+      <c r="D36">
         <v>25</v>
       </c>
-      <c r="E40">
-        <v>4</v>
-      </c>
-      <c r="F40">
-        <f>(C40*D40*E40*$C$37)/8</f>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <f>(C36*D36*E36*$C$32)/8</f>
         <v>4000</v>
       </c>
-      <c r="G40">
-        <f t="shared" ref="G40:G43" si="4">C40*$G$37</f>
-        <v>320</v>
-      </c>
-      <c r="H40">
-        <f t="shared" ref="H40:H43" si="5">D40*$G$37</f>
-        <v>200</v>
-      </c>
-      <c r="I40">
-        <f>$B$1/G40</f>
-        <v>2</v>
-      </c>
-      <c r="J40">
-        <f>$C$1/H40</f>
-        <v>2</v>
-      </c>
-      <c r="K40">
-        <f t="shared" ref="K40:K43" si="6">$B$2-F40</f>
-        <v>61536</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="C41">
-        <v>80</v>
-      </c>
-      <c r="D41">
-        <v>25</v>
-      </c>
-      <c r="E41">
-        <v>2</v>
-      </c>
-      <c r="F41">
-        <f>(C41*D41*E41*$C$37)/8</f>
-        <v>4000</v>
-      </c>
-      <c r="G41">
+      <c r="G36">
         <f t="shared" si="4"/>
         <v>640</v>
       </c>
-      <c r="H41">
+      <c r="H36">
         <f t="shared" si="5"/>
         <v>200</v>
       </c>
-      <c r="I41">
-        <f>$B$1/G41</f>
-        <v>1</v>
-      </c>
-      <c r="J41">
-        <f>$C$1/H41</f>
-        <v>2</v>
-      </c>
-      <c r="K41">
+      <c r="I36">
+        <f>$B$1/G36</f>
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <f>$C$1/H36</f>
+        <v>2</v>
+      </c>
+      <c r="K36">
         <f t="shared" si="6"/>
         <v>61536</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B42">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37">
         <v>3</v>
       </c>
-      <c r="C42">
+      <c r="C37">
         <v>80</v>
       </c>
-      <c r="D42">
+      <c r="D37">
         <v>50</v>
       </c>
-      <c r="E42">
-        <v>2</v>
-      </c>
-      <c r="F42">
-        <f>(C42*D42*E42*$C$37)/8</f>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <f>(C37*D37*E37*$C$32)/8</f>
         <v>8000</v>
       </c>
-      <c r="G42">
+      <c r="G37">
         <f t="shared" si="4"/>
         <v>640</v>
       </c>
-      <c r="H42">
+      <c r="H37">
         <f t="shared" si="5"/>
         <v>400</v>
       </c>
-      <c r="I42">
-        <f>$B$1/G42</f>
-        <v>1</v>
-      </c>
-      <c r="J42">
-        <f>$C$1/H42</f>
-        <v>1</v>
-      </c>
-      <c r="K42">
+      <c r="I37">
+        <f>$B$1/G37</f>
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <f>$C$1/H37</f>
+        <v>1</v>
+      </c>
+      <c r="K37">
         <f t="shared" si="6"/>
         <v>57536</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <v>4</v>
-      </c>
-      <c r="C43">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
         <v>80</v>
       </c>
-      <c r="D43">
+      <c r="D38">
         <v>50</v>
       </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43">
-        <f>(C43*D43*E43*$C$37)/8</f>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <f>(C38*D38*E38*$C$32)/8</f>
         <v>4000</v>
       </c>
-      <c r="G43">
+      <c r="G38">
         <f t="shared" si="4"/>
         <v>640</v>
       </c>
-      <c r="H43">
+      <c r="H38">
         <f t="shared" si="5"/>
         <v>400</v>
       </c>
-      <c r="I43">
-        <f>$B$1/G43</f>
-        <v>1</v>
-      </c>
-      <c r="J43">
-        <f>$C$1/H43</f>
-        <v>1</v>
-      </c>
-      <c r="K43">
+      <c r="I38">
+        <f>$B$1/G38</f>
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <f>$C$1/H38</f>
+        <v>1</v>
+      </c>
+      <c r="K38">
         <f t="shared" si="6"/>
         <v>61536</v>
       </c>
@@ -1746,10 +1596,10 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="G33:H33"/>
   </mergeCells>
-  <conditionalFormatting sqref="F7:F34">
+  <conditionalFormatting sqref="F7:F29">
     <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
       <formula>$B$2</formula>
     </cfRule>
@@ -1759,27 +1609,27 @@
       <formula>$B$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D34">
+  <conditionalFormatting sqref="D6:D29">
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>COUNTIF($K$5:$K$9,D6) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C34">
+  <conditionalFormatting sqref="C6:C29">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>COUNTIF($J$5:$J$9,C6) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:H34">
+  <conditionalFormatting sqref="G6:H29">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>NOT(INT(G6) = G6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
+  <conditionalFormatting sqref="F34">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>$B$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
+  <conditionalFormatting sqref="F35">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>$B$2</formula>
     </cfRule>

</xml_diff>

<commit_message>
Initial CRT Emulation and Clock
</commit_message>
<xml_diff>
--- a/Documentation/GraphicsModes.xlsx
+++ b/Documentation/GraphicsModes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>W</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>Left</t>
+  </si>
+  <si>
+    <t>Gfx Size</t>
+  </si>
+  <si>
+    <t>Txt Size</t>
+  </si>
+  <si>
+    <t>Gfx.S</t>
+  </si>
+  <si>
+    <t>Lines</t>
   </si>
 </sst>
 </file>
@@ -123,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -131,29 +143,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -535,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2332A2-3074-4648-AFA2-D28A6BF7FB4B}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,10 +556,19 @@
         <v>9</v>
       </c>
       <c r="B1">
-        <v>640</v>
+        <v>320</v>
       </c>
       <c r="C1">
-        <v>400</v>
+        <v>256</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1">
+        <v>320</v>
+      </c>
+      <c r="G1">
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -571,6 +579,25 @@
         <f>2^16</f>
         <v>65536</v>
       </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>320</v>
+      </c>
+      <c r="G2">
+        <v>256</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <f>(C1-G1)/2</f>
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -600,176 +627,164 @@
       <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J5">
-        <v>640</v>
-      </c>
-      <c r="K5">
-        <v>400</v>
-      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>80</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f>(C6*D6*E6*$C$4)/8</f>
-        <v>4000</v>
+        <v>640</v>
       </c>
       <c r="G6" s="4">
-        <f>$B$1/C6</f>
-        <v>8</v>
+        <f>$F$1/C6</f>
+        <v>4</v>
       </c>
       <c r="H6" s="4">
-        <f>$C$1/D6</f>
-        <v>8</v>
+        <f>$G$1/D6</f>
+        <v>4</v>
       </c>
       <c r="I6">
         <f>$B$2-F6</f>
-        <v>61536</v>
-      </c>
-      <c r="J6">
-        <v>320</v>
-      </c>
-      <c r="K6">
-        <v>200</v>
+        <v>64896</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>80</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F29" si="0">(C7*D7*E7*$C$4)/8</f>
-        <v>2000</v>
+        <f t="shared" ref="F7:F14" si="0">(C7*D7*E7*$C$4)/8</f>
+        <v>1280</v>
       </c>
       <c r="G7" s="4">
-        <f t="shared" ref="G7:G29" si="1">$B$1/C7</f>
-        <v>8</v>
+        <f t="shared" ref="G7:G14" si="1">$F$1/C7</f>
+        <v>4</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" ref="H7:H29" si="2">$C$1/D7</f>
-        <v>8</v>
+        <f t="shared" ref="H7:H14" si="2">$G$1/D7</f>
+        <v>4</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I29" si="3">$B$2-F7</f>
-        <v>63536</v>
+        <f t="shared" ref="I7:I14" si="3">$B$2-F7</f>
+        <v>64256</v>
       </c>
       <c r="J7">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="K7">
-        <v>100</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>80</v>
       </c>
       <c r="D8">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>2560</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>64536</v>
+        <v>62976</v>
       </c>
       <c r="J8">
+        <v>160</v>
+      </c>
+      <c r="K8">
         <v>128</v>
-      </c>
-      <c r="K8">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5">
-        <v>80</v>
-      </c>
-      <c r="D9" s="5">
-        <v>50</v>
-      </c>
-      <c r="E9" s="5">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>160</v>
+      </c>
+      <c r="D9">
+        <v>128</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="G9" s="6">
+        <v>2560</v>
+      </c>
+      <c r="G9" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="H9" s="6">
+        <v>2</v>
+      </c>
+      <c r="H9" s="4">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>65036</v>
+        <v>62976</v>
       </c>
       <c r="J9">
         <v>80</v>
       </c>
       <c r="K9">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10">
+        <v>160</v>
+      </c>
+      <c r="D10">
         <v>128</v>
       </c>
-      <c r="D10">
-        <v>80</v>
-      </c>
       <c r="E10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
@@ -777,11 +792,11 @@
       </c>
       <c r="G10" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H10" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
@@ -790,575 +805,152 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11">
+        <v>160</v>
+      </c>
+      <c r="D11">
         <v>128</v>
       </c>
-      <c r="D11">
-        <v>80</v>
-      </c>
       <c r="E11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>2560</v>
+        <v>10240</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>62976</v>
+        <v>55296</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5">
-        <v>128</v>
-      </c>
-      <c r="D12" s="5">
-        <v>80</v>
-      </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>320</v>
+      </c>
+      <c r="D12">
+        <v>256</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="0"/>
-        <v>1280</v>
-      </c>
-      <c r="G12" s="6">
+        <v>10240</v>
+      </c>
+      <c r="G12" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="H12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>64256</v>
+        <v>55296</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D13">
-        <v>80</v>
+        <v>256</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>6400</v>
+        <v>20480</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H13" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>59136</v>
+        <v>45056</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="D14">
-        <v>80</v>
+        <v>256</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>3200</v>
+        <v>40960</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f t="shared" si="3"/>
-        <v>62336</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" s="5">
-        <v>160</v>
-      </c>
-      <c r="D15" s="5">
-        <v>80</v>
-      </c>
-      <c r="E15" s="5">
-        <v>1</v>
-      </c>
-      <c r="F15" s="5">
-        <f t="shared" si="0"/>
-        <v>1600</v>
-      </c>
-      <c r="G15" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H15" s="6">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="3"/>
-        <v>63936</v>
-      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16">
-        <v>160</v>
-      </c>
-      <c r="D16">
-        <v>100</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>8000</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H16" s="4">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="3"/>
-        <v>57536</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17">
-        <v>160</v>
-      </c>
-      <c r="D17">
-        <v>100</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H17" s="4">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="3"/>
-        <v>61536</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5">
-        <v>160</v>
-      </c>
-      <c r="D18" s="5">
-        <v>100</v>
-      </c>
-      <c r="E18" s="5">
-        <v>1</v>
-      </c>
-      <c r="F18" s="5">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="G18" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H18" s="6">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="3"/>
-        <v>63536</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>18</v>
-      </c>
-      <c r="C19">
-        <v>320</v>
-      </c>
-      <c r="D19">
-        <v>100</v>
-      </c>
-      <c r="E19">
-        <v>4</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>16000</v>
-      </c>
-      <c r="G19" s="4">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H19" s="4">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="3"/>
-        <v>49536</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>19</v>
-      </c>
-      <c r="C20">
-        <v>320</v>
-      </c>
-      <c r="D20">
-        <v>100</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>8000</v>
-      </c>
-      <c r="G20" s="4">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H20" s="4">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="3"/>
-        <v>57536</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21" s="5">
-        <v>320</v>
-      </c>
-      <c r="D21" s="5">
-        <v>100</v>
-      </c>
-      <c r="E21" s="5">
-        <v>1</v>
-      </c>
-      <c r="F21" s="5">
-        <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="G21" s="6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H21" s="6">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="3"/>
-        <v>61536</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22">
-        <v>320</v>
-      </c>
-      <c r="D22">
-        <v>200</v>
-      </c>
-      <c r="E22">
-        <v>4</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>32000</v>
-      </c>
-      <c r="G22" s="4">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H22" s="4">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="3"/>
-        <v>33536</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23">
-        <v>320</v>
-      </c>
-      <c r="D23">
-        <v>200</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>16000</v>
-      </c>
-      <c r="G23" s="4">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H23" s="4">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="3"/>
-        <v>49536</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>23</v>
-      </c>
-      <c r="C24" s="5">
-        <v>320</v>
-      </c>
-      <c r="D24" s="5">
-        <v>200</v>
-      </c>
-      <c r="E24" s="5">
-        <v>1</v>
-      </c>
-      <c r="F24" s="5">
-        <f t="shared" si="0"/>
-        <v>8000</v>
-      </c>
-      <c r="G24" s="6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="H24" s="6">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="3"/>
-        <v>57536</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>24</v>
-      </c>
-      <c r="C25">
-        <v>640</v>
-      </c>
-      <c r="D25">
-        <v>200</v>
-      </c>
-      <c r="E25">
-        <v>4</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>64000</v>
-      </c>
-      <c r="G25" s="4">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H25" s="4">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="3"/>
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>25</v>
-      </c>
-      <c r="C26">
-        <v>640</v>
-      </c>
-      <c r="D26">
-        <v>200</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>32000</v>
-      </c>
-      <c r="G26" s="4">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H26" s="4">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="3"/>
-        <v>33536</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>26</v>
-      </c>
-      <c r="C27" s="5">
-        <v>640</v>
-      </c>
-      <c r="D27" s="5">
-        <v>200</v>
-      </c>
-      <c r="E27" s="5">
-        <v>1</v>
-      </c>
-      <c r="F27" s="5">
-        <f t="shared" si="0"/>
-        <v>16000</v>
-      </c>
-      <c r="G27" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H27" s="6">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="3"/>
-        <v>49536</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>27</v>
-      </c>
-      <c r="C28">
-        <v>640</v>
-      </c>
-      <c r="D28">
-        <v>400</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="0"/>
-        <v>64000</v>
-      </c>
-      <c r="G28" s="4">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H28" s="4">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="3"/>
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>28</v>
-      </c>
-      <c r="C29">
-        <v>640</v>
-      </c>
-      <c r="D29">
-        <v>400</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="0"/>
-        <v>32000</v>
-      </c>
-      <c r="G29" s="4">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H29" s="4">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="3"/>
-        <v>33536</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -1391,14 +983,14 @@
       <c r="F33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G33" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7" t="s">
+      <c r="H33" s="5"/>
+      <c r="I33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J33" s="7"/>
+      <c r="J33" s="5"/>
       <c r="K33" s="2" t="s">
         <v>16</v>
       </c>
@@ -1408,37 +1000,37 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D34">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F34">
         <f>(C34*D34*E34*$C$32)/8</f>
-        <v>800</v>
+        <v>160</v>
       </c>
       <c r="G34">
         <f>C34*$G$32</f>
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="H34">
         <f>D34*$G$32</f>
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="I34">
-        <f>$B$1/G34</f>
+        <f>$F$2/G34</f>
         <v>4</v>
       </c>
       <c r="J34">
-        <f>$C$1/H34</f>
-        <v>5</v>
+        <f>$G$2/H34</f>
+        <v>4</v>
       </c>
       <c r="K34">
         <f>$B$2-F34</f>
-        <v>64736</v>
+        <v>65376</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
@@ -1446,37 +1038,37 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D35">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F35">
         <f>(C35*D35*E35*$C$32)/8</f>
-        <v>4000</v>
+        <v>640</v>
       </c>
       <c r="G35">
-        <f t="shared" ref="G35:G38" si="4">C35*$G$32</f>
-        <v>320</v>
+        <f t="shared" ref="G35:G36" si="4">C35*$G$32</f>
+        <v>160</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35:H38" si="5">D35*$G$32</f>
-        <v>200</v>
+        <f t="shared" ref="H35:H36" si="5">D35*$G$32</f>
+        <v>128</v>
       </c>
       <c r="I35">
-        <f>$B$1/G35</f>
+        <f t="shared" ref="I35:I36" si="6">$F$2/G35</f>
         <v>2</v>
       </c>
       <c r="J35">
-        <f>$C$1/H35</f>
+        <f t="shared" ref="J35:J36" si="7">$G$2/H35</f>
         <v>2</v>
       </c>
       <c r="K35">
-        <f t="shared" ref="K35:K38" si="6">$B$2-F35</f>
-        <v>61536</v>
+        <f t="shared" ref="K35:K36" si="8">$B$2-F35</f>
+        <v>64896</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -1484,113 +1076,37 @@
         <v>2</v>
       </c>
       <c r="C36">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D36">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E36">
         <v>2</v>
       </c>
       <c r="F36">
         <f>(C36*D36*E36*$C$32)/8</f>
-        <v>4000</v>
+        <v>2560</v>
       </c>
       <c r="G36">
         <f t="shared" si="4"/>
-        <v>640</v>
+        <v>320</v>
       </c>
       <c r="H36">
         <f t="shared" si="5"/>
-        <v>200</v>
+        <v>256</v>
       </c>
       <c r="I36">
-        <f>$B$1/G36</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J36">
-        <f>$C$1/H36</f>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="K36">
-        <f t="shared" si="6"/>
-        <v>61536</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="C37">
-        <v>80</v>
-      </c>
-      <c r="D37">
-        <v>50</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37">
-        <f>(C37*D37*E37*$C$32)/8</f>
-        <v>8000</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="4"/>
-        <v>640</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="5"/>
-        <v>400</v>
-      </c>
-      <c r="I37">
-        <f>$B$1/G37</f>
-        <v>1</v>
-      </c>
-      <c r="J37">
-        <f>$C$1/H37</f>
-        <v>1</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="6"/>
-        <v>57536</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38">
-        <v>4</v>
-      </c>
-      <c r="C38">
-        <v>80</v>
-      </c>
-      <c r="D38">
-        <v>50</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <f>(C38*D38*E38*$C$32)/8</f>
-        <v>4000</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="4"/>
-        <v>640</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="5"/>
-        <v>400</v>
-      </c>
-      <c r="I38">
-        <f>$B$1/G38</f>
-        <v>1</v>
-      </c>
-      <c r="J38">
-        <f>$C$1/H38</f>
-        <v>1</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="6"/>
-        <v>61536</v>
+        <f t="shared" si="8"/>
+        <v>62976</v>
       </c>
     </row>
   </sheetData>
@@ -1609,12 +1125,12 @@
       <formula>$B$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D29">
+  <conditionalFormatting sqref="D6:D21 E21">
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>COUNTIF($K$5:$K$9,D6) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C29">
+  <conditionalFormatting sqref="C6:C21">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>COUNTIF($J$5:$J$9,C6) = 0</formula>
     </cfRule>

</xml_diff>

<commit_message>
(From earlier stream) NumPlanes configurable, bugfixes with mmu
</commit_message>
<xml_diff>
--- a/Documentation/GraphicsModes.xlsx
+++ b/Documentation/GraphicsModes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>W</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Lines</t>
+  </si>
+  <si>
+    <t>TileMem</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,6 +865,10 @@
         <f t="shared" si="3"/>
         <v>55296</v>
       </c>
+      <c r="J12">
+        <f>I12-$J$17</f>
+        <v>45056</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13">
@@ -892,6 +899,10 @@
         <f t="shared" si="3"/>
         <v>45056</v>
       </c>
+      <c r="J13">
+        <f t="shared" ref="J13:J14" si="4">I13-$J$17</f>
+        <v>34816</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -922,6 +933,10 @@
         <f t="shared" si="3"/>
         <v>24576</v>
       </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>14336</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G15" s="4"/>
@@ -931,26 +946,32 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17">
+        <v>10240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H21" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -1051,23 +1072,23 @@
         <v>640</v>
       </c>
       <c r="G35">
-        <f t="shared" ref="G35:G36" si="4">C35*$G$32</f>
+        <f t="shared" ref="G35:G36" si="5">C35*$G$32</f>
         <v>160</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35:H36" si="5">D35*$G$32</f>
+        <f t="shared" ref="H35:H36" si="6">D35*$G$32</f>
         <v>128</v>
       </c>
       <c r="I35">
-        <f t="shared" ref="I35:I36" si="6">$F$2/G35</f>
+        <f t="shared" ref="I35:I36" si="7">$F$2/G35</f>
         <v>2</v>
       </c>
       <c r="J35">
-        <f t="shared" ref="J35:J36" si="7">$G$2/H35</f>
+        <f t="shared" ref="J35:J36" si="8">$G$2/H35</f>
         <v>2</v>
       </c>
       <c r="K35">
-        <f t="shared" ref="K35:K36" si="8">$B$2-F35</f>
+        <f t="shared" ref="K35:K36" si="9">$B$2-F35</f>
         <v>64896</v>
       </c>
     </row>
@@ -1089,23 +1110,23 @@
         <v>2560</v>
       </c>
       <c r="G36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>320</v>
       </c>
       <c r="H36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>256</v>
       </c>
       <c r="I36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="K36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>62976</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New CPU core building tools. Started on SDL2 based Player.
</commit_message>
<xml_diff>
--- a/Documentation/GraphicsModes.xlsx
+++ b/Documentation/GraphicsModes.xlsx
@@ -19,11 +19,12 @@
     <sheet name="Sprite Flags" sheetId="6" r:id="rId5"/>
     <sheet name="Scanlines" sheetId="8" r:id="rId6"/>
     <sheet name="Cycles" sheetId="9" r:id="rId7"/>
-    <sheet name="Scanline Cycles" sheetId="15" r:id="rId8"/>
-    <sheet name="Graphics Memory Layout" sheetId="17" r:id="rId9"/>
-    <sheet name="Fetch Cycles Possibilities 2" sheetId="16" r:id="rId10"/>
-    <sheet name="Fetch Cycle Possibilities" sheetId="12" r:id="rId11"/>
-    <sheet name="Bus Cycles" sheetId="18" r:id="rId12"/>
+    <sheet name="Bus Cycles2" sheetId="19" r:id="rId8"/>
+    <sheet name="Scanline Cycles" sheetId="15" r:id="rId9"/>
+    <sheet name="Graphics Memory Layout" sheetId="17" r:id="rId10"/>
+    <sheet name="Fetch Cycles Possibilities 2" sheetId="16" r:id="rId11"/>
+    <sheet name="Fetch Cycle Possibilities" sheetId="12" r:id="rId12"/>
+    <sheet name="Bus Cycles Clocks" sheetId="18" r:id="rId13"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="325">
   <si>
     <t>Rows</t>
   </si>
@@ -958,6 +959,87 @@
   </si>
   <si>
     <t>ns</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>CPU bus cycles for upper vblank</t>
+  </si>
+  <si>
+    <t>Video Cycles per Frame</t>
+  </si>
+  <si>
+    <t>Bus Cycles per Video Cycle</t>
+  </si>
+  <si>
+    <t>Timing</t>
+  </si>
+  <si>
+    <t>Upper V-Blank</t>
+  </si>
+  <si>
+    <t>Lower V-Blank</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Start of Frame</t>
+  </si>
+  <si>
+    <t>End of Frame</t>
+  </si>
+  <si>
+    <t>Bus Cycles</t>
+  </si>
+  <si>
+    <t>CPU Cycles</t>
+  </si>
+  <si>
+    <t>Video Cycles</t>
+  </si>
+  <si>
+    <t>Hardware Accurate</t>
+  </si>
+  <si>
+    <t>Alternate</t>
+  </si>
+  <si>
+    <t>Graphics 0.25</t>
+  </si>
+  <si>
+    <t>Graphics 0</t>
+  </si>
+  <si>
+    <t>Graphics 0.5</t>
+  </si>
+  <si>
+    <t>Graphics 1.</t>
+  </si>
+  <si>
+    <t>Processsor 0</t>
+  </si>
+  <si>
+    <t>Processsor 1</t>
+  </si>
+  <si>
+    <t>Processsor 2</t>
+  </si>
+  <si>
+    <t>Processsor 3</t>
+  </si>
+  <si>
+    <t>Processsor 4</t>
+  </si>
+  <si>
+    <t>Processsor 5</t>
+  </si>
+  <si>
+    <t>Processsor 6</t>
+  </si>
+  <si>
+    <t>Processsor 7</t>
   </si>
 </sst>
 </file>
@@ -1287,7 +1369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1536,6 +1618,78 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1560,78 +1714,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2287,6 +2370,61 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D249BFBA-0298-4E66-B6A4-15BEF4579859}">
+  <dimension ref="E7:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="7" spans="5:12">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="5:12">
+      <c r="E8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0AD1171-1535-4BA0-8B37-79E704CFFF23}">
   <dimension ref="G2:I5"/>
   <sheetViews>
@@ -2322,7 +2460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E3BE9C6-4F5A-493E-963D-DE54AE108FC3}">
   <dimension ref="H1:O41"/>
   <sheetViews>
@@ -3074,21 +3212,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC17AB6-C9C6-40A9-9F62-724E8567381D}">
-  <dimension ref="B2:N18"/>
+  <dimension ref="B1:P18"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="M18" sqref="M3:M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="9.5703125" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="1" spans="2:16">
+      <c r="M1" t="s">
+        <v>311</v>
+      </c>
+      <c r="P1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16">
       <c r="C2" t="s">
         <v>65</v>
       </c>
@@ -3099,7 +3246,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:16">
       <c r="B3" s="1" t="s">
         <v>254</v>
       </c>
@@ -3117,8 +3264,11 @@
       <c r="M3" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="4" spans="2:14">
+      <c r="P3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16">
       <c r="B4" s="1" t="s">
         <v>290</v>
       </c>
@@ -3136,8 +3286,11 @@
       <c r="M4" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="5" spans="2:14">
+      <c r="P4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16">
       <c r="B5" s="1" t="s">
         <v>255</v>
       </c>
@@ -3151,109 +3304,151 @@
       <c r="M5" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="6" spans="2:14">
+      <c r="P5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16">
       <c r="K6">
         <v>3</v>
       </c>
       <c r="M6" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="7" spans="2:14">
+      <c r="P6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16">
       <c r="K7">
         <v>4</v>
       </c>
       <c r="M7" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="8" spans="2:14">
+      <c r="P7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16">
       <c r="K8">
         <v>5</v>
       </c>
       <c r="M8" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="9" spans="2:14">
+      <c r="P8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
       <c r="K9">
         <v>6</v>
       </c>
       <c r="M9" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="10" spans="2:14">
+      <c r="P9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16">
       <c r="K10">
         <v>7</v>
       </c>
       <c r="M10" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="11" spans="2:14">
+      <c r="P10" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16">
       <c r="K11">
         <v>8</v>
       </c>
       <c r="M11" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="12" spans="2:14">
+      <c r="P11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
       <c r="K12">
         <v>9</v>
       </c>
       <c r="M12" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="13" spans="2:14">
+      <c r="P12" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16">
       <c r="K13">
         <v>10</v>
       </c>
       <c r="M13" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="14" spans="2:14">
+      <c r="P13" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
       <c r="K14">
         <v>11</v>
       </c>
       <c r="M14" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="15" spans="2:14">
+      <c r="P14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
       <c r="K15">
         <v>12</v>
       </c>
       <c r="M15" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="16" spans="2:14">
+      <c r="P15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
       <c r="K16">
         <v>13</v>
       </c>
       <c r="M16" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="17" spans="11:13">
+      <c r="P16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="11:16">
       <c r="K17">
         <v>14</v>
       </c>
       <c r="M17" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="18" spans="11:13">
+      <c r="P17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="11:16">
       <c r="K18">
         <v>15</v>
       </c>
       <c r="M18" t="s">
         <v>290</v>
+      </c>
+      <c r="P18" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -5724,8 +5919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE63064-49DB-413A-8491-CD941DDB6868}">
   <dimension ref="C2:L42"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5734,7 +5929,8 @@
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30.42578125" customWidth="1"/>
@@ -5895,7 +6091,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:10">
       <c r="C17" s="2" t="s">
         <v>81</v>
       </c>
@@ -5907,7 +6103,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:10">
       <c r="C18" s="2" t="s">
         <v>84</v>
       </c>
@@ -5919,7 +6115,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:10">
       <c r="C19" s="2" t="s">
         <v>73</v>
       </c>
@@ -5931,7 +6127,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:10">
       <c r="C20" s="2" t="s">
         <v>71</v>
       </c>
@@ -5943,7 +6139,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:10">
       <c r="C21" s="2" t="s">
         <v>72</v>
       </c>
@@ -5955,7 +6151,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:10">
       <c r="C22" s="2" t="s">
         <v>74</v>
       </c>
@@ -5967,7 +6163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:10">
       <c r="C23" s="2" t="s">
         <v>75</v>
       </c>
@@ -5979,7 +6175,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:10">
       <c r="C24" s="2" t="s">
         <v>76</v>
       </c>
@@ -5991,7 +6187,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:10">
       <c r="C25" s="2" t="s">
         <v>77</v>
       </c>
@@ -6002,8 +6198,22 @@
       <c r="E25" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="3:7">
+      <c r="G25" t="s">
+        <v>299</v>
+      </c>
+      <c r="H25">
+        <f>D25*8</f>
+        <v>14240</v>
+      </c>
+      <c r="I25">
+        <f>H25*D38</f>
+        <v>1778406.5477332312</v>
+      </c>
+      <c r="J25" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10">
       <c r="C26" s="2" t="s">
         <v>82</v>
       </c>
@@ -6014,8 +6224,15 @@
       <c r="E26" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="3:7">
+      <c r="I26">
+        <f>I25/10^9</f>
+        <v>1.7784065477332311E-3</v>
+      </c>
+      <c r="J26" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10">
       <c r="C28" t="s">
         <v>182</v>
       </c>
@@ -6023,8 +6240,19 @@
         <f>D11*D8</f>
         <v>1000896</v>
       </c>
-    </row>
-    <row r="29" spans="3:7">
+      <c r="H28">
+        <f>D11*8</f>
+        <v>159744</v>
+      </c>
+      <c r="I28">
+        <f>H28*D38</f>
+        <v>19950124.688279305</v>
+      </c>
+      <c r="J28" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10">
       <c r="D29">
         <f>D28/1000000</f>
         <v>1.000896</v>
@@ -6036,8 +6264,15 @@
         <f>(1/D8)/D11</f>
         <v>9.9910480209732085E-7</v>
       </c>
-    </row>
-    <row r="30" spans="3:7">
+      <c r="I29">
+        <f>I28/10^9</f>
+        <v>1.9950124688279305E-2</v>
+      </c>
+      <c r="J29" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10">
       <c r="F30">
         <f>F29*10^9</f>
         <v>999.10480209732088</v>
@@ -6181,6 +6416,175 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49EDA878-BCE1-47EE-BB50-E6B432BA9DD5}">
+  <dimension ref="C1:O9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:15">
+      <c r="J1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2" spans="3:15">
+      <c r="C2" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15">
+      <c r="D3">
+        <f>Cycles!D11</f>
+        <v>19968</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f>J3/2</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>J3/16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15">
+      <c r="I4" s="132" t="s">
+        <v>303</v>
+      </c>
+      <c r="J4">
+        <f>Cycles!D25*D6</f>
+        <v>28480</v>
+      </c>
+      <c r="K4">
+        <f>J4-J3</f>
+        <v>28480</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L6" si="0">J4/2</f>
+        <v>14240</v>
+      </c>
+      <c r="M4">
+        <f>L4-L3</f>
+        <v>14240</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N6" si="1">J4/16</f>
+        <v>1780</v>
+      </c>
+      <c r="O4">
+        <f>N4-N3</f>
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15">
+      <c r="C5" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="J5">
+        <f>Cycles!D23*D6</f>
+        <v>290624</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K7" si="2">J5-J4</f>
+        <v>262144</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>145312</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M6" si="3">L5-L4</f>
+        <v>131072</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>18164</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:O6" si="4">N5-N4</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15">
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="J6">
+        <f>D3*D6</f>
+        <v>319488</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>28864</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>159744</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>14432</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>19968</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15">
+      <c r="C8" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15">
+      <c r="D9">
+        <f>D3*D6</f>
+        <v>319488</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE06816-33F1-403B-888C-1BEF60C28D1F}">
   <dimension ref="A1:BB92"/>
   <sheetViews>
@@ -6214,156 +6618,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="51" customFormat="1" ht="26.25">
-      <c r="E1" s="115" t="s">
+      <c r="E1" s="118" t="s">
         <v>175</v>
       </c>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="115" t="s">
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="118" t="s">
         <v>231</v>
       </c>
-      <c r="L1" s="116"/>
-      <c r="M1" s="116"/>
-      <c r="N1" s="116"/>
-      <c r="O1" s="116"/>
-      <c r="P1" s="116"/>
-      <c r="Q1" s="116"/>
-      <c r="R1" s="116"/>
-      <c r="S1" s="116"/>
-      <c r="T1" s="116"/>
-      <c r="U1" s="116"/>
-      <c r="V1" s="116"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="118"/>
-      <c r="Y1" s="118"/>
-      <c r="Z1" s="118"/>
-      <c r="AA1" s="118"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
+      <c r="P1" s="119"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="120"/>
+      <c r="X1" s="121"/>
+      <c r="Y1" s="121"/>
+      <c r="Z1" s="121"/>
+      <c r="AA1" s="121"/>
     </row>
     <row r="2" spans="1:54" ht="15" customHeight="1">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="108" t="s">
         <v>242</v>
       </c>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="112" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="109" t="s">
         <v>243</v>
       </c>
-      <c r="D2" s="120" t="s">
+      <c r="D2" s="106" t="s">
         <v>232</v>
       </c>
-      <c r="E2" s="111" t="s">
+      <c r="E2" s="122" t="s">
         <v>159</v>
       </c>
-      <c r="F2" s="119" t="s">
+      <c r="F2" s="109" t="s">
         <v>234</v>
       </c>
-      <c r="G2" s="119" t="s">
+      <c r="G2" s="109" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="119" t="s">
+      <c r="H2" s="109" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="119" t="s">
+      <c r="I2" s="109" t="s">
         <v>176</v>
       </c>
-      <c r="J2" s="119" t="s">
+      <c r="J2" s="109" t="s">
         <v>173</v>
       </c>
-      <c r="K2" s="108" t="s">
+      <c r="K2" s="114" t="s">
         <v>144</v>
       </c>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="110"/>
+      <c r="L2" s="115"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="116"/>
       <c r="O2" s="72"/>
-      <c r="P2" s="108" t="s">
+      <c r="P2" s="114" t="s">
         <v>180</v>
       </c>
-      <c r="Q2" s="109"/>
-      <c r="R2" s="109"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="108" t="s">
+      <c r="Q2" s="115"/>
+      <c r="R2" s="115"/>
+      <c r="S2" s="116"/>
+      <c r="T2" s="114" t="s">
         <v>172</v>
       </c>
-      <c r="U2" s="109"/>
-      <c r="V2" s="109"/>
-      <c r="W2" s="110"/>
-      <c r="X2" s="108" t="s">
+      <c r="U2" s="115"/>
+      <c r="V2" s="115"/>
+      <c r="W2" s="116"/>
+      <c r="X2" s="114" t="s">
         <v>177</v>
       </c>
-      <c r="Y2" s="109"/>
-      <c r="Z2" s="109"/>
-      <c r="AA2" s="110"/>
+      <c r="Y2" s="115"/>
+      <c r="Z2" s="115"/>
+      <c r="AA2" s="116"/>
     </row>
     <row r="3" spans="1:54">
-      <c r="A3" s="119"/>
-      <c r="B3" s="128"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
-      <c r="J3" s="119"/>
-      <c r="K3" s="111">
-        <v>0</v>
-      </c>
-      <c r="L3" s="113">
-        <v>1</v>
-      </c>
-      <c r="M3" s="113">
+      <c r="A3" s="109"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="122">
+        <v>0</v>
+      </c>
+      <c r="L3" s="108">
+        <v>1</v>
+      </c>
+      <c r="M3" s="108">
         <v>2</v>
       </c>
-      <c r="N3" s="112">
+      <c r="N3" s="123">
         <v>3</v>
       </c>
       <c r="O3" s="73"/>
-      <c r="P3" s="111">
+      <c r="P3" s="122">
         <v>0</v>
       </c>
       <c r="Q3" s="73"/>
       <c r="R3" s="73"/>
-      <c r="S3" s="112">
+      <c r="S3" s="123">
         <v>3</v>
       </c>
-      <c r="T3" s="102" t="s">
+      <c r="T3" s="126" t="s">
         <v>275</v>
       </c>
-      <c r="U3" s="103"/>
-      <c r="V3" s="103"/>
-      <c r="W3" s="104"/>
-      <c r="X3" s="102" t="s">
+      <c r="U3" s="127"/>
+      <c r="V3" s="127"/>
+      <c r="W3" s="128"/>
+      <c r="X3" s="126" t="s">
         <v>260</v>
       </c>
-      <c r="Y3" s="103"/>
-      <c r="Z3" s="103"/>
-      <c r="AA3" s="104"/>
+      <c r="Y3" s="127"/>
+      <c r="Z3" s="127"/>
+      <c r="AA3" s="128"/>
     </row>
     <row r="4" spans="1:54" s="19" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A4" s="119"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="119"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="114"/>
-      <c r="M4" s="114"/>
-      <c r="N4" s="112"/>
+      <c r="A4" s="109"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="122"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="117"/>
+      <c r="N4" s="123"/>
       <c r="O4" s="73"/>
-      <c r="P4" s="111"/>
+      <c r="P4" s="122"/>
       <c r="Q4" s="73"/>
       <c r="R4" s="73"/>
-      <c r="S4" s="112"/>
+      <c r="S4" s="123"/>
       <c r="T4" s="75">
         <v>0</v>
       </c>
@@ -6453,12 +6857,12 @@
       <c r="Q5" s="71"/>
       <c r="R5" s="71"/>
       <c r="S5" s="61"/>
-      <c r="T5" s="105"/>
-      <c r="U5" s="105"/>
+      <c r="T5" s="129"/>
+      <c r="U5" s="129"/>
       <c r="V5" s="55"/>
       <c r="W5" s="55"/>
-      <c r="X5" s="106"/>
-      <c r="Y5" s="107"/>
+      <c r="X5" s="130"/>
+      <c r="Y5" s="131"/>
       <c r="Z5" s="62"/>
       <c r="AA5" s="83"/>
     </row>
@@ -6691,8 +7095,8 @@
       </c>
       <c r="T9" s="34"/>
       <c r="U9" s="23"/>
-      <c r="V9" s="100"/>
-      <c r="W9" s="100"/>
+      <c r="V9" s="124"/>
+      <c r="W9" s="124"/>
       <c r="X9" s="81" t="s">
         <v>271</v>
       </c>
@@ -6799,14 +7203,14 @@
       <c r="U11" s="23"/>
       <c r="V11" s="23"/>
       <c r="W11" s="23"/>
-      <c r="X11" s="124" t="s">
+      <c r="X11" s="103" t="s">
         <v>244</v>
       </c>
-      <c r="Y11" s="125"/>
-      <c r="Z11" s="125" t="s">
+      <c r="Y11" s="104"/>
+      <c r="Z11" s="104" t="s">
         <v>245</v>
       </c>
-      <c r="AA11" s="126"/>
+      <c r="AA11" s="105"/>
     </row>
     <row r="12" spans="1:54">
       <c r="A12" t="str">
@@ -6848,14 +7252,14 @@
       <c r="U12" s="23"/>
       <c r="V12" s="23"/>
       <c r="W12" s="23"/>
-      <c r="X12" s="124" t="s">
+      <c r="X12" s="103" t="s">
         <v>246</v>
       </c>
-      <c r="Y12" s="125"/>
-      <c r="Z12" s="125" t="s">
+      <c r="Y12" s="104"/>
+      <c r="Z12" s="104" t="s">
         <v>249</v>
       </c>
-      <c r="AA12" s="126"/>
+      <c r="AA12" s="105"/>
     </row>
     <row r="13" spans="1:54">
       <c r="A13" t="str">
@@ -6897,14 +7301,14 @@
       <c r="U13" s="23"/>
       <c r="V13" s="23"/>
       <c r="W13" s="23"/>
-      <c r="X13" s="124" t="s">
+      <c r="X13" s="103" t="s">
         <v>247</v>
       </c>
-      <c r="Y13" s="125"/>
-      <c r="Z13" s="125" t="s">
+      <c r="Y13" s="104"/>
+      <c r="Z13" s="104" t="s">
         <v>250</v>
       </c>
-      <c r="AA13" s="126"/>
+      <c r="AA13" s="105"/>
     </row>
     <row r="14" spans="1:54">
       <c r="A14" t="str">
@@ -6946,14 +7350,14 @@
       <c r="U14" s="23"/>
       <c r="V14" s="23"/>
       <c r="W14" s="23"/>
-      <c r="X14" s="124" t="s">
+      <c r="X14" s="103" t="s">
         <v>248</v>
       </c>
-      <c r="Y14" s="125"/>
-      <c r="Z14" s="125" t="s">
+      <c r="Y14" s="104"/>
+      <c r="Z14" s="104" t="s">
         <v>251</v>
       </c>
-      <c r="AA14" s="126"/>
+      <c r="AA14" s="105"/>
     </row>
     <row r="15" spans="1:54" ht="50.25" customHeight="1">
       <c r="A15" t="str">
@@ -9563,12 +9967,12 @@
       <c r="J57" s="6">
         <v>0</v>
       </c>
-      <c r="K57" s="124" t="s">
+      <c r="K57" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="L57" s="125"/>
-      <c r="M57" s="125"/>
-      <c r="N57" s="126"/>
+      <c r="L57" s="104"/>
+      <c r="M57" s="104"/>
+      <c r="N57" s="105"/>
       <c r="O57" s="70"/>
       <c r="P57" s="77" t="s">
         <v>235</v>
@@ -9626,12 +10030,12 @@
       <c r="J58" s="37">
         <v>0</v>
       </c>
-      <c r="K58" s="124" t="s">
+      <c r="K58" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="L58" s="125"/>
-      <c r="M58" s="125"/>
-      <c r="N58" s="126"/>
+      <c r="L58" s="104"/>
+      <c r="M58" s="104"/>
+      <c r="N58" s="105"/>
       <c r="O58" s="70"/>
       <c r="P58" s="77" t="s">
         <v>235</v>
@@ -9689,12 +10093,12 @@
       <c r="J59" s="37">
         <v>0</v>
       </c>
-      <c r="K59" s="124" t="s">
+      <c r="K59" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="L59" s="125"/>
-      <c r="M59" s="125"/>
-      <c r="N59" s="126"/>
+      <c r="L59" s="104"/>
+      <c r="M59" s="104"/>
+      <c r="N59" s="105"/>
       <c r="O59" s="70"/>
       <c r="P59" s="77" t="s">
         <v>235</v>
@@ -9752,12 +10156,12 @@
       <c r="J60" s="37">
         <v>0</v>
       </c>
-      <c r="K60" s="124" t="s">
+      <c r="K60" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="L60" s="125"/>
-      <c r="M60" s="125"/>
-      <c r="N60" s="126"/>
+      <c r="L60" s="104"/>
+      <c r="M60" s="104"/>
+      <c r="N60" s="105"/>
       <c r="O60" s="70"/>
       <c r="P60" s="77" t="s">
         <v>235</v>
@@ -9815,12 +10219,12 @@
       <c r="J61" s="37">
         <v>0</v>
       </c>
-      <c r="K61" s="124" t="s">
+      <c r="K61" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="L61" s="125"/>
-      <c r="M61" s="125"/>
-      <c r="N61" s="126"/>
+      <c r="L61" s="104"/>
+      <c r="M61" s="104"/>
+      <c r="N61" s="105"/>
       <c r="O61" s="70"/>
       <c r="P61" s="77" t="s">
         <v>235</v>
@@ -9878,12 +10282,12 @@
       <c r="J62" s="37">
         <v>0</v>
       </c>
-      <c r="K62" s="124" t="s">
+      <c r="K62" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="L62" s="125"/>
-      <c r="M62" s="125"/>
-      <c r="N62" s="126"/>
+      <c r="L62" s="104"/>
+      <c r="M62" s="104"/>
+      <c r="N62" s="105"/>
       <c r="O62" s="70"/>
       <c r="P62" s="77" t="s">
         <v>235</v>
@@ -9941,12 +10345,12 @@
       <c r="J63" s="37">
         <v>0</v>
       </c>
-      <c r="K63" s="124" t="s">
+      <c r="K63" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="L63" s="125"/>
-      <c r="M63" s="125"/>
-      <c r="N63" s="126"/>
+      <c r="L63" s="104"/>
+      <c r="M63" s="104"/>
+      <c r="N63" s="105"/>
       <c r="O63" s="70"/>
       <c r="P63" s="77" t="s">
         <v>235</v>
@@ -10004,12 +10408,12 @@
       <c r="J64" s="37">
         <v>0</v>
       </c>
-      <c r="K64" s="124" t="s">
+      <c r="K64" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="L64" s="125"/>
-      <c r="M64" s="125"/>
-      <c r="N64" s="126"/>
+      <c r="L64" s="104"/>
+      <c r="M64" s="104"/>
+      <c r="N64" s="105"/>
       <c r="O64" s="70"/>
       <c r="P64" s="77" t="s">
         <v>235</v>
@@ -10067,12 +10471,12 @@
       <c r="J65" s="37">
         <v>0</v>
       </c>
-      <c r="K65" s="124" t="s">
+      <c r="K65" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="L65" s="125"/>
-      <c r="M65" s="125"/>
-      <c r="N65" s="126"/>
+      <c r="L65" s="104"/>
+      <c r="M65" s="104"/>
+      <c r="N65" s="105"/>
       <c r="O65" s="70"/>
       <c r="P65" s="77" t="s">
         <v>235</v>
@@ -10130,12 +10534,12 @@
       <c r="J66" s="37">
         <v>0</v>
       </c>
-      <c r="K66" s="124" t="s">
+      <c r="K66" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="L66" s="125"/>
-      <c r="M66" s="125"/>
-      <c r="N66" s="126"/>
+      <c r="L66" s="104"/>
+      <c r="M66" s="104"/>
+      <c r="N66" s="105"/>
       <c r="O66" s="70"/>
       <c r="P66" s="77" t="s">
         <v>235</v>
@@ -10193,12 +10597,12 @@
       <c r="J67" s="37">
         <v>0</v>
       </c>
-      <c r="K67" s="124" t="s">
+      <c r="K67" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="L67" s="125"/>
-      <c r="M67" s="125"/>
-      <c r="N67" s="126"/>
+      <c r="L67" s="104"/>
+      <c r="M67" s="104"/>
+      <c r="N67" s="105"/>
       <c r="O67" s="70"/>
       <c r="P67" s="77" t="s">
         <v>235</v>
@@ -10256,12 +10660,12 @@
       <c r="J68" s="39">
         <v>0</v>
       </c>
-      <c r="K68" s="129" t="s">
+      <c r="K68" s="100" t="s">
         <v>235</v>
       </c>
-      <c r="L68" s="130"/>
-      <c r="M68" s="130"/>
-      <c r="N68" s="131"/>
+      <c r="L68" s="101"/>
+      <c r="M68" s="101"/>
+      <c r="N68" s="102"/>
       <c r="O68" s="68"/>
       <c r="P68" s="79" t="s">
         <v>235</v>
@@ -10293,12 +10697,12 @@
       <c r="AA68" s="80"/>
     </row>
     <row r="69" spans="1:27" ht="29.25" thickBot="1">
-      <c r="A69" s="122" t="s">
+      <c r="A69" s="110" t="s">
         <v>241</v>
       </c>
-      <c r="B69" s="122"/>
-      <c r="C69" s="122"/>
-      <c r="D69" s="123"/>
+      <c r="B69" s="110"/>
+      <c r="C69" s="110"/>
+      <c r="D69" s="111"/>
       <c r="E69" s="54"/>
       <c r="F69" s="50"/>
       <c r="G69" s="50"/>
@@ -10423,16 +10827,16 @@
       <c r="Q77" s="69"/>
       <c r="R77" s="69"/>
       <c r="S77" s="76"/>
-      <c r="T77" s="101" t="s">
+      <c r="T77" s="125" t="s">
         <v>166</v>
       </c>
-      <c r="U77" s="101"/>
-      <c r="V77" s="101"/>
-      <c r="W77" s="101"/>
-      <c r="X77" s="101"/>
-      <c r="Y77" s="101"/>
-      <c r="Z77" s="101"/>
-      <c r="AA77" s="101"/>
+      <c r="U77" s="125"/>
+      <c r="V77" s="125"/>
+      <c r="W77" s="125"/>
+      <c r="X77" s="125"/>
+      <c r="Y77" s="125"/>
+      <c r="Z77" s="125"/>
+      <c r="AA77" s="125"/>
     </row>
     <row r="78" spans="1:27">
       <c r="F78" s="32"/>
@@ -10449,16 +10853,16 @@
       <c r="Q78" s="69"/>
       <c r="R78" s="69"/>
       <c r="S78" s="76"/>
-      <c r="T78" s="101" t="s">
+      <c r="T78" s="125" t="s">
         <v>167</v>
       </c>
-      <c r="U78" s="101"/>
-      <c r="V78" s="101"/>
-      <c r="W78" s="101"/>
-      <c r="X78" s="101"/>
-      <c r="Y78" s="101"/>
-      <c r="Z78" s="101"/>
-      <c r="AA78" s="101"/>
+      <c r="U78" s="125"/>
+      <c r="V78" s="125"/>
+      <c r="W78" s="125"/>
+      <c r="X78" s="125"/>
+      <c r="Y78" s="125"/>
+      <c r="Z78" s="125"/>
+      <c r="AA78" s="125"/>
     </row>
     <row r="80" spans="1:27">
       <c r="T80" s="93" t="s">
@@ -10492,13 +10896,34 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="K68:N68"/>
-    <mergeCell ref="X11:Y11"/>
-    <mergeCell ref="Z11:AA11"/>
-    <mergeCell ref="X12:Y12"/>
-    <mergeCell ref="Z12:AA12"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="T78:AA78"/>
+    <mergeCell ref="T77:AA77"/>
+    <mergeCell ref="X3:AA3"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="X14:Y14"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="K1:W1"/>
+    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="K3:K4"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A69:D69"/>
@@ -10515,91 +10940,15 @@
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="K66:N66"/>
     <mergeCell ref="K67:N67"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="K1:W1"/>
-    <mergeCell ref="X1:AA1"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="T2:W2"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="T78:AA78"/>
-    <mergeCell ref="T77:AA77"/>
-    <mergeCell ref="X3:AA3"/>
-    <mergeCell ref="T3:W3"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="X14:Y14"/>
-    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="K68:N68"/>
+    <mergeCell ref="X11:Y11"/>
+    <mergeCell ref="Z11:AA11"/>
+    <mergeCell ref="X12:Y12"/>
+    <mergeCell ref="Z12:AA12"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="Z13:AA13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D249BFBA-0298-4E66-B6A4-15BEF4579859}">
-  <dimension ref="E7:L8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="7" spans="5:12">
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-      <c r="K7">
-        <v>6</v>
-      </c>
-      <c r="L7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="5:12">
-      <c r="E8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8" t="s">
-        <v>163</v>
-      </c>
-      <c r="H8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>